<commit_message>
new field added in territory import
</commit_message>
<xml_diff>
--- a/Presentation/AVPolyPack.API/FormatFiles/Template_Territories.xlsx
+++ b/Presentation/AVPolyPack.API/FormatFiles/Template_Territories.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>IsActive</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>DistrictName</t>
+  </si>
+  <si>
+    <t>CountryName</t>
   </si>
 </sst>
 </file>
@@ -381,7 +384,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -389,36 +392,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
       <formula1>"True,False"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>